<commit_message>
Zistenie smeru pohybu z poschodia (zber ludi)
Na poschodiach sa system rozhodne ci a ak ano ktorym smerom sa ma
pohnut, beruc do uvahy privolavace na poschodiach a tlacidla v kabine.
(Zatial neberie do uvahy signaly DPK a DOORCLSD) Vytah tiez zatial
nezastai na poschodi, kde je volba v sachte opacnym smerom aj ked v jeho
smere ziadna ina volba nie je. Bola tiez opravena chyba pri zistovani,
ci na poschodi zastavit.
</commit_message>
<xml_diff>
--- a/Testovanie.xlsx
+++ b/Testovanie.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>Test</t>
   </si>
@@ -130,6 +130,12 @@
   </si>
   <si>
     <t>FLOOR2 - ERR_2SPOM_C</t>
+  </si>
+  <si>
+    <t>4 to 1</t>
+  </si>
+  <si>
+    <t>Na dvojek zastavilo s hlaskou ERR_1SPOM_C</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
   <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -697,6 +703,18 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>36</v>
+      </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Implementacia Zotavenia sa z chybovych stavov
Boli implemenovane stavy ERROR a ERROR2 a prechody do nich zo stavov
ERR_1SPOM_C, ERR_2SPOM_C, ERR_ZAST_C, ERR_SKRD a ERR_SKRH. Taktiez bolo
implementovane obsluzenie prerusenia casovaca, no neuspesne (kod
zakomentavany)
</commit_message>
<xml_diff>
--- a/Testovanie.xlsx
+++ b/Testovanie.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5532"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5532" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hárok1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
+    <sheet name="Požiadavky" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="56">
   <si>
     <t>Test</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Prislo az na 1. posch a mysli si, ze je na druhom</t>
   </si>
   <si>
-    <t>Detekcia ERR_ZAST_C, ERR_2_SPOM_C, Kalibracia, uistim sa, ze som na poschodi</t>
-  </si>
-  <si>
     <t>1 to 2, 2 to 3</t>
   </si>
   <si>
@@ -136,6 +133,66 @@
   </si>
   <si>
     <t>Na dvojek zastavilo s hlaskou ERR_1SPOM_C</t>
+  </si>
+  <si>
+    <t>Číslo</t>
+  </si>
+  <si>
+    <t>Akonáhle preťažím kabínu, spomalím.</t>
+  </si>
+  <si>
+    <t>Ak je kabína preťažená, nepohnem sa z poschodia.</t>
+  </si>
+  <si>
+    <t>Zastaviť teba nielen keď je privolávač v tvojom smere, ale aj keď už v tomto smere nič viac zvolené nie je.</t>
+  </si>
+  <si>
+    <t>Ak idem rýchlo, nemôžem na poschodí zastaviť!</t>
+  </si>
+  <si>
+    <t>Spomaľ aj keď pochádza voľba zo šachty!</t>
+  </si>
+  <si>
+    <t>Ak nespomalím pred poschodím pri preťažení,  nemôžem na ňom zastaviť!</t>
+  </si>
+  <si>
+    <t>Vyriešiť kabínové dvere.</t>
+  </si>
+  <si>
+    <t>Vyriešiť tlačidlo STOP.</t>
+  </si>
+  <si>
+    <t>Zotavenie sa zo stavov</t>
+  </si>
+  <si>
+    <t>Nepohni sa, ak je kabína preťažená!</t>
+  </si>
+  <si>
+    <t>Ak nie je v kabíne nič stlačené, ale je v nej osoba (osoby) kabína sa nesmie pohnúť.</t>
+  </si>
+  <si>
+    <t>Chcem s osobou trhnúť hneď po zatvorení dverí?</t>
+  </si>
+  <si>
+    <t>POZOR na relatívne skoky! (použi SJMP namiesto JMP)</t>
+  </si>
+  <si>
+    <t>POZOR! Zálohuj všetky registre do STACKu pri rutinách!</t>
+  </si>
+  <si>
+    <t>Vyrieš svetlo v kabíne (povedal by som nech svieti vždy keď sa hýbe a keď stojí tak iba v prípade, že je aktívny signál DPK, DPZK, alebo DP</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Pridať stav spomalenia (už tam sa rozhodnem či stáť alebo nie)</t>
+  </si>
+  <si>
+    <t>POZOR</t>
+  </si>
+  <si>
+    <t>Ak sú na poschodí otvorené kabínové dvere nepohni sa! Potom keď už vyhodnotíš, že sa môžes pohnúť počkaj ešte chvíľočku. To ti zabezpečí úctu a slávu.  (že ťa netrhne hneď ako zatvoríš dvere)</t>
   </si>
 </sst>
 </file>
@@ -172,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -180,11 +237,46 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normálna" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -496,7 +588,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -664,7 +756,7 @@
     </row>
     <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -673,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L8" s="1" t="s">
         <v>5</v>
@@ -684,7 +776,7 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -693,7 +785,7 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="1" t="s">
         <v>5</v>
@@ -704,7 +796,7 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -713,7 +805,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>5</v>
@@ -750,34 +842,230 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="76.5546875" customWidth="1"/>
+    <col min="2" max="2" width="87.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="3.77734375" customWidth="1"/>
+    <col min="4" max="4" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="B4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
-        <v>30</v>
+      <c r="B12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:D1048576">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+      <formula>"OK"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+      <formula>"?"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"POZOR"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="5" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>